<commit_message>
modified test.txt.txt and demo files
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CA7812-0F23-46E3-B425-AE4913E1FA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2446742E-026C-493B-91C2-71370206D0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>dvv</t>
+  </si>
+  <si>
+    <t>wa</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -337,10 +351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -360,6 +374,21 @@
         <v>678</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>